<commit_message>
Change two dates from CET to GMT
</commit_message>
<xml_diff>
--- a/Proposal/Sporting Events 2012 with Names.xlsx
+++ b/Proposal/Sporting Events 2012 with Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgree\Documents\Python Scripts\Project\git-rep\london-power-analysis\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A183C8EC-6A02-4BDB-9E2F-D53EA874ACDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7304D559-02FA-4CF4-AB52-A4B2B348A1CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58905" yWindow="2520" windowWidth="20640" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -990,7 +990,7 @@
         <v>43535</v>
       </c>
       <c r="F22" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="G22" t="s">
         <v>30</v>
@@ -1019,7 +1019,7 @@
         <v>43507</v>
       </c>
       <c r="F23" s="2">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G23" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Corrected start times of some soccer games
</commit_message>
<xml_diff>
--- a/Proposal/Sporting Events 2012 with Names.xlsx
+++ b/Proposal/Sporting Events 2012 with Names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Data Analytics Bootcamp\Projects\london-power-analysis\Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgree\Documents\Python Scripts\Project\git-rep\london-power-analysis\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E1FF167-30CF-465C-AB18-93141929037E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C0EF7C-F7AD-486D-A087-115ACA10DF7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,26 +534,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.41796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.41796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="83.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
@@ -583,7 +583,7 @@
       </c>
       <c r="M1" s="4"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>23</v>
       </c>
@@ -609,7 +609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -635,7 +635,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -661,7 +661,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -687,7 +687,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -713,7 +713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -742,7 +742,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -771,7 +771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -797,7 +797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -808,7 +808,7 @@
         <v>43627</v>
       </c>
       <c r="F14" s="2">
-        <v>0.79166666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>
@@ -823,7 +823,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -834,7 +834,7 @@
         <v>43635</v>
       </c>
       <c r="F15" s="2">
-        <v>0.90625</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="G15" t="s">
         <v>32</v>
@@ -849,7 +849,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -860,7 +860,7 @@
         <v>43631</v>
       </c>
       <c r="F16" s="2">
-        <v>0.91666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
@@ -868,14 +868,14 @@
       <c r="H16">
         <v>14.3</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="K16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -886,7 +886,7 @@
         <v>43640</v>
       </c>
       <c r="F17" s="2">
-        <v>0.90625</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
@@ -901,7 +901,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -927,7 +927,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -953,7 +953,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -982,7 +982,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -1131,8 +1131,9 @@
   <hyperlinks>
     <hyperlink ref="J8" r:id="rId1" xr:uid="{A58A6D26-AC09-45AD-9320-A90DD7C19A54}"/>
     <hyperlink ref="L22" r:id="rId2" xr:uid="{77CE65B4-4D0A-4C11-AA76-9AB8DB7DDFE8}"/>
+    <hyperlink ref="J16" r:id="rId3" xr:uid="{03ECCE09-05C2-4221-B3C7-0AE724BC7609}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More corrections to start times
</commit_message>
<xml_diff>
--- a/Proposal/Sporting Events 2012 with Names.xlsx
+++ b/Proposal/Sporting Events 2012 with Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgree\Documents\Python Scripts\Project\git-rep\london-power-analysis\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C0EF7C-F7AD-486D-A087-115ACA10DF7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0210BC8D-5738-415D-89B7-2008B63A0072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60150" yWindow="120" windowWidth="18900" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -594,7 +594,7 @@
         <v>43569</v>
       </c>
       <c r="F3" s="2">
-        <v>0.67708333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -646,7 +646,7 @@
         <v>43654</v>
       </c>
       <c r="F7" s="2">
-        <v>0.64583333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="G7" t="s">
         <v>30</v>
@@ -672,7 +672,7 @@
         <v>43653</v>
       </c>
       <c r="F8" s="2">
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="G8" t="s">
         <v>30</v>
@@ -698,13 +698,13 @@
         <v>43590</v>
       </c>
       <c r="F10" s="2">
-        <v>0.71875</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
       <c r="H10">
-        <v>11.2</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="J10" t="s">
         <v>35</v>
@@ -782,7 +782,7 @@
         <v>43522</v>
       </c>
       <c r="F13" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="G13" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Adjusted to show kick-off times and not broadcast times
</commit_message>
<xml_diff>
--- a/Proposal/Sporting Events 2012 with Names.xlsx
+++ b/Proposal/Sporting Events 2012 with Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgree\Documents\Python Scripts\Project\git-rep\london-power-analysis\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0210BC8D-5738-415D-89B7-2008B63A0072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47453B80-E9BA-4AE3-9D46-70DCA0914F6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60150" yWindow="120" windowWidth="18900" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60795" yWindow="1260" windowWidth="18900" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -594,7 +594,7 @@
         <v>43569</v>
       </c>
       <c r="F3" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -646,7 +646,7 @@
         <v>43654</v>
       </c>
       <c r="F7" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G7" t="s">
         <v>30</v>
@@ -672,7 +672,7 @@
         <v>43653</v>
       </c>
       <c r="F8" s="2">
-        <v>0.5625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G8" t="s">
         <v>30</v>
@@ -698,7 +698,7 @@
         <v>43590</v>
       </c>
       <c r="F10" s="2">
-        <v>0.63541666666666663</v>
+        <v>0.71875</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
@@ -782,7 +782,7 @@
         <v>43522</v>
       </c>
       <c r="F13" s="2">
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G13" t="s">
         <v>34</v>
@@ -964,7 +964,7 @@
         <v>43800</v>
       </c>
       <c r="F21" s="2">
-        <v>0.6875</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="G21" t="s">
         <v>44</v>

</xml_diff>